<commit_message>
Updated URLs and amounts
</commit_message>
<xml_diff>
--- a/STM32F407 era/Samlet BOM.xlsx
+++ b/STM32F407 era/Samlet BOM.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henri\Documents\GitHub\g5-pcb\STM32F407 era\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\backup skrivebord\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
     <sheet name="H-Bridge" sheetId="9" r:id="rId9"/>
     <sheet name="Relay" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="357">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="367">
   <si>
     <t>COM-TC</t>
   </si>
@@ -722,9 +722,6 @@
     <t>https://www.digikey.dk/product-detail/en/wurth-electronics-inc/9774050151R/732-7095-1-ND/5320700</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/amp-te-connectivity/1717468-3/ddr-smt-ra-200way/dp/2250075</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/c-k-components/pts645sl43-2-lfs/tactile-switch-spst-0-05a-12vdc/dp/2435161</t>
   </si>
   <si>
@@ -755,21 +752,12 @@
     <t>http://dk.farnell.com/molex/36638-0002/header-cmc-single-port-r-a-48way/dp/1830389?MER=sy-me-pd-mi-acce</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/multicomp/2214s-06sg-85/connector-receptacle-pcb-2-54mm/dp/1593488</t>
-  </si>
-  <si>
     <t>https://dk.rs-online.com/web/p/dioder-ensretter-og-schottky-dioder/7384778/</t>
   </si>
   <si>
     <t>https://dk.rs-online.com/web/p/batteriholdere/2197948/</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/greenpar-te-connectivity/1-1478204-0/rf-coaxial-bnc-straight-jack-50ohm/dp/1056271</t>
-  </si>
-  <si>
-    <t>http://dk.farnell.com/walsin/0603b104k250ct/capacitor-mlcc-x7r-0-1uf-25v-0603/dp/2496833</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/kemet/c0603c103k5rac7081/cap-mlcc-x7r-0-01uf-50v-0603/dp/2522596</t>
   </si>
   <si>
@@ -818,12 +806,6 @@
     <t>http://dk.farnell.com/murata/grm21br61e475ma12l/cap-mlcc-x5r-4-7uf-25v-0805/dp/2362111</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/tdk/c2012x5r1a476m125ac/cap-mlcc-x5r-47uf-10v-0805/dp/2211186RL</t>
-  </si>
-  <si>
-    <t>http://dk.farnell.com/murata/grm31cf50j107ze01l/cap-mlcc-y5v-100uf-6-3v-1206/dp/2362115</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/murata/grm31cr60j157me11l/capacitor-mlcc-x5r-150uf-6-3v/dp/2494474</t>
   </si>
   <si>
@@ -839,9 +821,6 @@
     <t>http://dk.farnell.com/iqd-frequency-products/lfxtal003215/crystal-12mhz/dp/9712950</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/qantek-technology-corporation/qcl6-00000f18b23b/crystal-6mhz-18pf-hc-49us/dp/2508445</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/multicomp/5504f1-09s-02a-03/receptacle-d-sub-tht-r-a-9way/dp/1848372</t>
   </si>
   <si>
@@ -851,21 +830,9 @@
     <t>http://dk.farnell.com/bourns/cd1607-b140lf/diode-schottky-1a-40v-1607/dp/1456527</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/nexperia/pmeg6010cej/schottky-rectifier-1a-60v-sod/dp/2575120</t>
-  </si>
-  <si>
-    <t>http://dk.farnell.com/nexperia/pdz3-3b-115/diode-zener-0-4w-3-3v-sod323/dp/1757856</t>
-  </si>
-  <si>
-    <t>https://dk.rs-online.com/web/p/lcd-monokrome-displays/7588765/</t>
-  </si>
-  <si>
     <t>https://www.digikey.dk/products/en?keywords=EA-LED78x64-W</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/e-switch/eg1218/slide-switch-spdt-0-2a-30vdc-th/dp/2787232</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/jst-japan-solderless-terminals/bm06b-srss-tb-lf-sn/header-smt-vertical-1mm-6way/dp/1679131</t>
   </si>
   <si>
@@ -887,9 +854,6 @@
     <t>http://dk.farnell.com/bourns/srn6045ta-680m/inductor-aec-q200-68uh-1-1a-20/dp/2616899</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/infineon/irf9332pbf/mosfet-p-ch-diode-30v-9-8a-so8/dp/1857354</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/jst-japan-solderless-terminals/s4b-ph-sm4-tb-lf-sn/header-smt-right-angle-2mm-4way/dp/9492631</t>
   </si>
   <si>
@@ -908,9 +872,6 @@
     <t>http://dk.farnell.com/littelfuse/01530008z/fuseholder-mini-pin/dp/9943790</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/stmicroelectronics/ld1117s33tr/v-reg-ldo-3-3v-smd-1117-sot-223/dp/1202826</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/stmicroelectronics/ld1117s50ctr/ic-v-reg-ldo-5v-smd/dp/1467780</t>
   </si>
   <si>
@@ -932,9 +893,6 @@
     <t>https://dk.rs-online.com/web/p/hall-effekt-sensor-icer/9237731/</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/on-semiconductor/mbr0520lt1g/diode-schottky-0-5a-20v-smc/dp/9556915</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/microchip/mcp2200-i-so/ic-usb2-0-to-uart-w-gpio-20soic/dp/1781148</t>
   </si>
   <si>
@@ -956,15 +914,6 @@
     <t>http://dk.farnell.com/camdenboss/ctb0708-2/terminal-block-wire-to-brd-1pos/dp/2315273</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/bi-technologies-tt-electronics/p090s-14t20br10k/rotary-potentiometer-10kohm-20/dp/1417123</t>
-  </si>
-  <si>
-    <t>http://dk.farnell.com/littelfuse/1206l020yr/fuse-ptc-resettable-24v-200ma/dp/2072173</t>
-  </si>
-  <si>
-    <t>http://dk.farnell.com/littelfuse/1812l110-16dr/fuse-ptc-resettable-16v-1-1a-1812/dp/2131406</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/c-k-components/pts645sm43smtr92lfs/switch-spst-0-05a-12vdc-smd-4/dp/2320087</t>
   </si>
   <si>
@@ -1007,9 +956,6 @@
     <t>http://dk.farnell.com/multicomp/mcwr06x27r0ftl/res-thick-film-27r-1-0-1w-0603/dp/2447316</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/multicomp/mc0063w0603160r4/res-thick-film-60r4-1-0-063w-0603/dp/1170666</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/multicomp/mcwr06x1000ftl/res-thick-film-100r-1-0-1w-0603/dp/2447227</t>
   </si>
   <si>
@@ -1052,12 +998,6 @@
     <t>http://dk.farnell.com/multicomp/mcwr06x152-jtl/res-thick-film-1k5-5-0-1w-0603/dp/2694727</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/multicomp/mcwr06x2003ftl/res-thick-film-200kohm-1-0-1w/dp/2447291</t>
-  </si>
-  <si>
-    <t>http://dk.farnell.com/multicomp/mcwr06x2002ftl/res-thick-film-20kohm-1-0-1w/dp/2447293</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/multicomp/mcwr06x2942ftl/res-thick-film-29k4-1-0-1w-0603/dp/2694813</t>
   </si>
   <si>
@@ -1070,9 +1010,6 @@
     <t>http://dk.farnell.com/multicomp/mcwr06x3832ftl/res-thick-film-38-3kohm-1-0-1w/dp/2447351</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/multicomp/mc0063w060313k24/res-thick-film-3k24-1-0-063w-0603/dp/1170839</t>
-  </si>
-  <si>
     <t>http://dk.farnell.com/multicomp/mcwr06x472-jtl/res-thick-film-4k7-5-0-1w-0603/dp/2694880</t>
   </si>
   <si>
@@ -1088,9 +1025,6 @@
     <t>http://dk.farnell.com/te-connectivity/crgs0805j10k/resistor-thick-film-10k-5-0805/dp/2531799</t>
   </si>
   <si>
-    <t>http://dk.farnell.com/multicomp/mcwf08p1005ftl/res-thick-film-10m-1-0-25w-0805/dp/2694099</t>
-  </si>
-  <si>
     <t>https://dk.rs-online.com/web/p/overflademontering-faste-modstande/2945040/</t>
   </si>
   <si>
@@ -1104,12 +1038,108 @@
   </si>
   <si>
     <t>http://dk.farnell.com/multicomp/bcw66g/transistor-npn-0-8a-45v-sot23/dp/1798056</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/product-detail/en/te-connectivity-amp-connectors/1717468-3/A114930-ND/1891351</t>
+  </si>
+  <si>
+    <t>7 haves</t>
+  </si>
+  <si>
+    <t>antal der skal bestilles</t>
+  </si>
+  <si>
+    <t>antal haves</t>
+  </si>
+  <si>
+    <t>tages ved kenneth</t>
+  </si>
+  <si>
+    <t>rigeligt</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/amp-te-connectivity/5-1634503-1/rf-coaxial-bnc-straight-jack-50ohm/dp/1020980</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/murata/grm21br61a476me15l/cap-mlcc-x5r-47uf-10v-0805/dp/2611939</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/panasonic-electronic-components/erj3ekf60r4v/res-thick-film-60r4-1-0-1w-0603/dp/2059280</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/multicomp/mcmr06x2002ftl/res-ceramic-20k-1-0-1w-0603/dp/2073421</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/walsin/wr06x3241ftl/res-thick-film-3k24-1-0-1w-0603/dp/2670754</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/panasonic-electronic-components/db2j41100l/diode-schottky-40v-smini2-f5-b/dp/2284946</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/on-semiconductor/mm3z3v3t1g/diode-zener-3-3v-0-2w/dp/1431198</t>
+  </si>
+  <si>
+    <t>https://www.digikey.dk/product-detail/en/electronic-assembly-gmbh/EA-DOGXL160W-7/1481-1099-ND/4896738</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/taiwan-semiconductor/ts2940cw-3-3-rp/v-reg-3-3v-smd-2940-sot-223-3/dp/7261403</t>
+  </si>
+  <si>
+    <t>ekstra nødstop</t>
+  </si>
+  <si>
+    <t>https://dk.rs-online.com/web/p/printstik-huse/2332753/?searchTerm=233-2753&amp;relevancy-data=636F3D3126696E3D4931384E525353746F636B4E756D6265724D504E266C753D656E266D6D3D6D61746368616C6C26706D3D5E283F69292852537C5253207C52532D293F5C647B337D285C73293F5B5C732D2F255C2E2C5D285C73293F5C647B332C347D2426706F3D313426736E3D592673743D52535F53544F434B5F4E554D4245522677633D4E4F4E45267573743D3233332D32373533267374613D3233333237353326</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/on-semiconductor/mbr0520l/diode-schottky-0-5a-20v-smd/dp/1467521</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/mercury-united-electronics/h49-6-000-18-30-50-40-85/crystal-6mhz-18pf-hc-49/dp/2509262?pf=112004383%2C112005728%2C110134637%2C110177854%2C110196752&amp;crystal-case=through-hole-10.8mm-x-4.5mm&amp;load-capacitance=16pf%7C18pf%7C20pf&amp;anyFilterApplied=true&amp;frequency-nom=6mhz&amp;ddkey=http%3Ada-DK%2FElement14_Denmark%2Fw%2Fc%2Fcrystals-oscillators%2Fcrystals</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/vishay/si4427bdy-t1-e3/mosfet-p-ch-30v-9-7a-soic/dp/2335312</t>
+  </si>
+  <si>
+    <t>conrad</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/alps/rk09k1130ah1/pot-rotary-10k-17mm-20/dp/1191725</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/multicomp/mc36207/fuse-ptc-reset-30v-200ma-smd/dp/1861187?MER=i-9b10-00001422</t>
+  </si>
+  <si>
+    <t>bestilt ved</t>
+  </si>
+  <si>
+    <t>digikey</t>
+  </si>
+  <si>
+    <t>https://dk.rs-online.com/web/p/sikringer-smd-tilbagestillende/6478207/</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/eao/84-5020-0040/switch-emergency-stop-1nc-240vac/dp/2787249</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/multicomp/mc0603f104z160ct/cap-mlcc-y5v-100nf-16v-0603/dp/1759017RL</t>
+  </si>
+  <si>
+    <t>https://dk.rs-online.com/web/p/keramiske-flerlags-kondensatorer/7492059/</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/alps/stsss9121/slide-switch-sp-2-pos-vert/dp/1123875</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/vishay/crcw060320k0fkea/res-thick-film-20k-1-0-1w-0603/dp/1469774</t>
+  </si>
+  <si>
+    <t>http://dk.farnell.com/welwyn/lr1206-r033fw/res-thick-film-0r033-1-0-5w-1206/dp/1099911</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1456,11 +1486,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I135"/>
+  <dimension ref="A1:X138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E137" sqref="E137"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,9 +1499,10 @@
     <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1500,36 +1531,45 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>338</v>
+      </c>
+      <c r="U2" t="s">
+        <v>337</v>
+      </c>
+      <c r="X2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1546,10 +1586,10 @@
         <v>227</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>(2*A2)+(2*C2)+(2*E2)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>223</v>
@@ -1557,11 +1597,17 @@
       <c r="E5" s="3" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <v>20</v>
+      </c>
+      <c r="X5" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>(Samlet!A2*'COM-TC'!A7)+(Dash!A7*Samlet!C2)+(Samlet!D2*Debug!A7)+(Samlet!E2*Dev!A15)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -1573,13 +1619,16 @@
         <v>22</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+      <c r="U6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>E2*Dev!A2</f>
-        <v>1</v>
+        <f>E2*Dev!A3</f>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>166</v>
@@ -1588,13 +1637,16 @@
         <v>167</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+      <c r="U7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>I2*Relay!A4</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
         <v>216</v>
@@ -1606,13 +1658,16 @@
         <v>216</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>I2*Relay!A5+G2*USB!A9</f>
-        <v>2</v>
+        <f>I2*Relay!A5+G2*USB!A2</f>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>217</v>
@@ -1624,10 +1679,13 @@
         <v>217</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+      <c r="U9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>H2*'H-Bridge'!A5</f>
         <v>0</v>
@@ -1642,13 +1700,16 @@
         <v>207</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="U10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>G2*USB!A10</f>
-        <v>4</v>
+        <f>G2*USB!A3</f>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>194</v>
@@ -1660,13 +1721,16 @@
         <v>195</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+      <c r="U11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>A2*'COM-TC'!A33</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>56</v>
@@ -1678,13 +1742,16 @@
         <v>57</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+      <c r="U12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>I2*Relay!A7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
         <v>218</v>
@@ -1696,13 +1763,16 @@
         <v>218</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>E2*Dev!A24</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
         <v>176</v>
@@ -1714,10 +1784,16 @@
         <v>177</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+      <c r="U14">
+        <v>8</v>
+      </c>
+      <c r="X14" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>178</v>
       </c>
@@ -1728,10 +1804,10 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>(E2*Dev!A3)+(Samlet!D2*Debug!A2)</f>
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="C16" t="s">
         <v>155</v>
@@ -1740,13 +1816,16 @@
         <v>156</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+      <c r="U16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>A2*'COM-TC'!A44</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
         <v>66</v>
@@ -1758,13 +1837,19 @@
         <v>67</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>238</v>
+      </c>
+      <c r="T17">
+        <v>2</v>
+      </c>
+      <c r="U17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>E2*Dev!A7</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
         <v>180</v>
@@ -1775,14 +1860,15 @@
       <c r="D18" t="s">
         <v>181</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="3"/>
+      <c r="U18" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>(A2*'COM-TC'!A43)+(Samlet!C2*Dash!A30)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
         <v>63</v>
@@ -1794,13 +1880,19 @@
         <v>65</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+      <c r="T19" t="s">
+        <v>340</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>B2*CPU!A15</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B20" t="s">
         <v>123</v>
@@ -1812,13 +1904,19 @@
         <v>125</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+      <c r="T20">
+        <v>10</v>
+      </c>
+      <c r="U20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>(D2*Debug!A10)+(Samlet!E2*Dev!A29)</f>
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
         <v>162</v>
@@ -1830,13 +1928,16 @@
         <v>163</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+      <c r="U21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>(A2*'COM-TC'!A8)+(Samlet!B2*CPU!A5)+(Samlet!C2*Dash!A8)+(Samlet!E2*Dev!A17)+(Samlet!F2*Tele!A7)+(Samlet!G2*USB!A4)</f>
-        <v>51</v>
+        <v>156</v>
       </c>
       <c r="B22" t="s">
         <v>23</v>
@@ -1848,13 +1949,16 @@
         <v>25</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+      <c r="U22">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>(A2*'COM-TC'!A13)+(Dash!A11)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
         <v>34</v>
@@ -1866,13 +1970,16 @@
         <v>25</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24">
         <f>(A2*'COM-TC'!A17)+(Samlet!C2*Dash!A14)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B24" t="s">
         <v>39</v>
@@ -1884,13 +1991,16 @@
         <v>25</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25">
         <f>B2*CPU!A6</f>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
         <v>109</v>
@@ -1902,13 +2012,16 @@
         <v>25</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+      <c r="U25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26">
         <f>(B2*CPU!A7)+(Samlet!F2*Tele!A10)+(Samlet!G2*USB!A11)</f>
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
         <v>110</v>
@@ -1920,13 +2033,16 @@
         <v>25</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>Samlet!G2*USB!A14</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
         <v>196</v>
@@ -1938,13 +2054,16 @@
         <v>25</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="U27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>B2*CPU!A9</f>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
         <v>114</v>
@@ -1956,13 +2075,16 @@
         <v>25</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29">
         <f>(A2*'COM-TC'!A29)+(Samlet!C2*Dash!A23)+(Samlet!D2*Debug!A8)+(Samlet!E2*Dev!A19)</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
         <v>53</v>
@@ -1974,13 +2096,16 @@
         <v>25</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+      <c r="U29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30">
         <f>(A2*'COM-TC'!A30)+(Samlet!C2*Dash!A24)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
         <v>54</v>
@@ -1992,13 +2117,16 @@
         <v>25</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>B2*CPU!A12</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
         <v>121</v>
@@ -2010,13 +2138,16 @@
         <v>25</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>B2*CPU!A14</f>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B32" t="s">
         <v>122</v>
@@ -2028,13 +2159,16 @@
         <v>25</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>(A2*'COM-TC'!A14)+(Samlet!H2*'H-Bridge'!A2)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
@@ -2046,13 +2180,16 @@
         <v>32</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="U33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34">
         <f>C2*Dash!A15</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
         <v>109</v>
@@ -2064,13 +2201,16 @@
         <v>32</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>C2*Dash!A17</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
         <v>138</v>
@@ -2082,13 +2222,16 @@
         <v>32</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+      <c r="U35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36">
         <f>(A2*'COM-TC'!A21)+(Samlet!H2*'H-Bridge'!A6)+(E2*Dev!A11)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B36" t="s">
         <v>42</v>
@@ -2100,13 +2243,16 @@
         <v>32</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="U36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37">
         <f>C2*Dash!A19</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B37" t="s">
         <v>139</v>
@@ -2118,13 +2264,16 @@
         <v>32</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="U37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38">
         <f>(A2*'COM-TC'!A28)+(Samlet!C2*Dash!A22)+(Samlet!F2*Tele!A12)+(Samlet!G2*USB!A16)</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B38" t="s">
         <v>52</v>
@@ -2136,13 +2285,16 @@
         <v>32</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+      <c r="U38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>(A2*'COM-TC'!A31)+(Samlet!C2*Dash!A25)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B39" t="s">
         <v>55</v>
@@ -2154,13 +2306,16 @@
         <v>32</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+      <c r="U39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40">
         <f>A2*'COM-TC'!A9</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B40" t="s">
         <v>26</v>
@@ -2172,13 +2327,16 @@
         <v>1206</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+      <c r="U40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41">
         <f>A2*'COM-TC'!A15</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B41" t="s">
         <v>37</v>
@@ -2190,10 +2348,13 @@
         <v>1206</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="U41">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42">
         <f>H2*'H-Bridge'!A4</f>
         <v>0</v>
@@ -2208,13 +2369,16 @@
         <v>206</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="U42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43">
         <f>B2*CPU!A11</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
         <v>118</v>
@@ -2226,13 +2390,16 @@
         <v>120</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+      <c r="U43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44">
         <f>B2*CPU!A8</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B44" t="s">
         <v>111</v>
@@ -2244,13 +2411,16 @@
         <v>113</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+      <c r="U44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45">
         <f>(F2*Tele!A9)+(Samlet!G2*USB!A6)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
         <v>185</v>
@@ -2262,13 +2432,16 @@
         <v>187</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="U45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46">
         <f>G2*USB!A18</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B46" t="s">
         <v>197</v>
@@ -2280,13 +2453,16 @@
         <v>187</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+      <c r="U46">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47">
         <f>D2*Debug!A4+Samlet!E2*Dev!A5</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C47" t="s">
         <v>158</v>
@@ -2295,13 +2471,16 @@
         <v>159</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+      <c r="U47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48">
         <f>D2*Debug!A5+Samlet!E2*Dev!A6</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
         <v>160</v>
@@ -2310,13 +2489,16 @@
         <v>161</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+      <c r="U48">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49">
         <f>I2*Relay!A2</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C49" t="s">
         <v>213</v>
@@ -2325,13 +2507,16 @@
         <v>214</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="U49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50">
         <f>A2*'COM-TC'!A2</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C50" t="s">
         <v>13</v>
@@ -2340,13 +2525,16 @@
         <v>14</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+      <c r="U50">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51">
         <f>B2*CPU!A10</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B51" t="s">
         <v>115</v>
@@ -2358,13 +2546,16 @@
         <v>117</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>347</v>
+      </c>
+      <c r="U51">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52">
         <f>C2*Dash!A32</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B52" t="s">
         <v>144</v>
@@ -2376,25 +2567,37 @@
         <v>144</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+      <c r="U52">
+        <v>2</v>
+      </c>
+      <c r="X52" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53">
         <f>A52</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B53" t="s">
         <v>224</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+      <c r="U53">
+        <v>2</v>
+      </c>
+      <c r="X53" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f>E2*Dev!A7</f>
-        <v>1</v>
+        <f>E2*Dev!A14</f>
+        <v>8</v>
       </c>
       <c r="C54" t="s">
         <v>168</v>
@@ -2403,13 +2606,16 @@
         <v>169</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+      <c r="U54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55">
         <f>A2*'COM-TC'!A45</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B55" t="s">
         <v>68</v>
@@ -2421,13 +2627,16 @@
         <v>68</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+      <c r="U55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56">
         <f>C2*Dash!A31</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B56" t="s">
         <v>141</v>
@@ -2439,13 +2648,19 @@
         <v>143</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+      <c r="T56">
+        <v>2</v>
+      </c>
+      <c r="U56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57">
         <f>A2*'COM-TC'!A46+Samlet!D2*Debug!A11+Samlet!E2*Dev!A30</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B57" t="s">
         <v>69</v>
@@ -2457,13 +2672,16 @@
         <v>70</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+      <c r="U57">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58">
         <f>I2*Relay!A8</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B58" t="s">
         <v>219</v>
@@ -2475,13 +2693,16 @@
         <v>220</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+      <c r="U58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59">
         <f>A2*'COM-TC'!A47</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B59" t="s">
         <v>71</v>
@@ -2493,13 +2714,16 @@
         <v>72</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+      <c r="U59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60">
         <f>A2*'COM-TC'!A60</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B60" t="s">
         <v>95</v>
@@ -2511,13 +2735,16 @@
         <v>97</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+      <c r="U60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61">
         <f>A2*'COM-TC'!A61+C2*Dash!A41</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B61" t="s">
         <v>98</v>
@@ -2529,13 +2756,16 @@
         <v>97</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>272</v>
+      </c>
+      <c r="U61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62">
         <f>A2*'COM-TC'!A48+Samlet!C2*Dash!A33</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B62" t="s">
         <v>73</v>
@@ -2547,13 +2777,16 @@
         <v>74</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+      <c r="U62">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63">
         <f>C2*Dash!A2</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C63" t="s">
         <v>132</v>
@@ -2562,13 +2795,16 @@
         <v>133</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+        <v>273</v>
+      </c>
+      <c r="U63">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64">
         <f>A2*'COM-TC'!A49+Samlet!C2*Dash!A34+Samlet!E2*Dev!A16</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B64" t="s">
         <v>75</v>
@@ -2580,13 +2816,16 @@
         <v>75</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+      <c r="U64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65">
         <f>C2*Dash!A3+Samlet!E2*Dev!A17</f>
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C65" t="s">
         <v>134</v>
@@ -2595,13 +2834,19 @@
         <v>135</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+      <c r="S65">
+        <v>50</v>
+      </c>
+      <c r="U65">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66">
         <f>E2*Dev!A18+Samlet!F2*Tele!A2+Samlet!I2*Relay!A3</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C66" t="s">
         <v>170</v>
@@ -2610,13 +2855,19 @@
         <v>171</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+      <c r="U66">
+        <v>30</v>
+      </c>
+      <c r="X66" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67">
         <f>F2*Tele!A3+Samlet!G2*USB!A10</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C67" t="s">
         <v>183</v>
@@ -2625,13 +2876,19 @@
         <v>184</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+      <c r="U67">
+        <v>15</v>
+      </c>
+      <c r="X67" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68">
         <f>I2*Relay!A9</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B68" t="s">
         <v>221</v>
@@ -2643,13 +2900,16 @@
         <v>222</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+      <c r="U68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69">
         <f>A2*'COM-TC'!A24+Samlet!E2*Dev!A19+Samlet!F2*Tele!A4+Samlet!G2*USB!A11</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B69" t="s">
         <v>45</v>
@@ -2661,13 +2921,16 @@
         <v>47</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+      <c r="U69">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70">
         <f>A2*'COM-TC'!A38+Samlet!E2*Dev!A20+Samlet!G2*USB!A12+H2*'H-Bridge'!A9</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B70" t="s">
         <v>60</v>
@@ -2679,13 +2942,16 @@
         <v>47</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+      <c r="U70">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71">
         <f>A2*'COM-TC'!A51+Samlet!E2*Dev!A21+Samlet!F2*Tele!A14</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B71" t="s">
         <v>79</v>
@@ -2697,13 +2963,19 @@
         <v>80</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+      <c r="T71">
+        <v>2</v>
+      </c>
+      <c r="U71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72">
         <f>A2*'COM-TC'!A50</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B72" t="s">
         <v>76</v>
@@ -2715,13 +2987,16 @@
         <v>78</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+      <c r="U72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73">
         <f>G2*USB!A13</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B73" t="s">
         <v>198</v>
@@ -2733,13 +3008,19 @@
         <v>199</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+      <c r="U73">
+        <v>3</v>
+      </c>
+      <c r="X73" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74">
         <f>A2*'COM-TC'!A52</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B74" t="s">
         <v>81</v>
@@ -2751,13 +3032,16 @@
         <v>82</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+      <c r="U74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75">
         <f>C2*Dash!A35</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B75" t="s">
         <v>145</v>
@@ -2769,13 +3053,19 @@
         <v>146</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+      <c r="U75">
+        <v>5</v>
+      </c>
+      <c r="X75" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76">
         <f>A2*'COM-TC'!A53</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B76" t="s">
         <v>83</v>
@@ -2787,13 +3077,22 @@
         <v>84</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+      <c r="S76" t="s">
+        <v>355</v>
+      </c>
+      <c r="U76">
+        <v>4</v>
+      </c>
+      <c r="X76" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77">
         <f>C2*Dash!A36</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B77" t="s">
         <v>147</v>
@@ -2805,13 +3104,16 @@
         <v>148</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+      <c r="U77">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78">
         <f>F2*Tele!A15+Samlet!G2*USB!A14</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B78" t="s">
         <v>188</v>
@@ -2823,13 +3125,19 @@
         <v>189</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+      <c r="U78">
+        <v>5</v>
+      </c>
+      <c r="X78" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79">
         <f>A2*'COM-TC'!A54</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B79" t="s">
         <v>85</v>
@@ -2841,13 +3149,19 @@
         <v>86</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+      <c r="U79">
+        <v>10</v>
+      </c>
+      <c r="X79" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80">
         <f>D2*Debug!A12+Samlet!E2*Dev!A22</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B80" t="s">
         <v>164</v>
@@ -2859,13 +3173,16 @@
         <v>165</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="U80">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81">
         <f>A2*'COM-TC'!A55+Samlet!E2*Dev!A23</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B81" t="s">
         <v>87</v>
@@ -2877,13 +3194,16 @@
         <v>87</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+        <v>289</v>
+      </c>
+      <c r="U81">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82">
         <f>A2*'COM-TC'!A57</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B82" t="s">
         <v>89</v>
@@ -2895,13 +3215,16 @@
         <v>91</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>290</v>
+      </c>
+      <c r="U82">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83">
         <f>C2*Dash!A4</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C83" t="s">
         <v>136</v>
@@ -2910,10 +3233,13 @@
         <v>19</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+      <c r="U83">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84">
         <f>H2*'H-Bridge'!A8</f>
         <v>0</v>
@@ -2928,13 +3254,16 @@
         <v>209</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="U84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85">
         <f>E2*Dev!A25</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C85" t="s">
         <v>172</v>
@@ -2943,13 +3272,16 @@
         <v>173</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+      <c r="U85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86">
         <f>B2*CPU!A2</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C86" t="s">
         <v>104</v>
@@ -2958,13 +3290,16 @@
         <v>1206</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+      <c r="U86">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87">
         <f>A2*'COM-TC'!A3+Samlet!C2*Dash!A5+Samlet!F2*Tele!A5</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C87" t="s">
         <v>15</v>
@@ -2973,13 +3308,16 @@
         <v>15</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+      <c r="U87">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88">
         <f>B2*CPU!A16</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B88" t="s">
         <v>126</v>
@@ -2991,13 +3329,16 @@
         <v>127</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+      <c r="U88" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89">
         <f>C2*Dash!A12</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B89">
         <v>15</v>
@@ -3009,13 +3350,16 @@
         <v>25</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+      <c r="U89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90">
         <f>G2*USB!A19</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B90">
         <v>27</v>
@@ -3027,13 +3371,16 @@
         <v>25</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+      <c r="U90">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91">
         <f>A2*'COM-TC'!A39+Samlet!C2*Dash!A27+Samlet!D2*Debug!A9+Samlet!E2*Dev!A26</f>
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B91">
         <v>60</v>
@@ -3045,13 +3392,16 @@
         <v>25</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+      <c r="U91">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92">
         <f>E2*Dev!A27</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B92">
         <v>100</v>
@@ -3063,13 +3413,16 @@
         <v>25</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+      <c r="U92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93">
         <f>A2*'COM-TC'!A20+Samlet!C2*Dash!A16</f>
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B93">
         <v>220</v>
@@ -3081,13 +3434,16 @@
         <v>25</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+      <c r="U93">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94">
         <f>E2*Dev!A28</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B94">
         <v>240</v>
@@ -3099,13 +3455,16 @@
         <v>25</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="U94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95">
         <f>F2*Tele!A11+Samlet!G2*USB!A20</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B95">
         <v>270</v>
@@ -3117,13 +3476,16 @@
         <v>25</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+      <c r="U95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96">
         <f>I2*Relay!A6</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B96">
         <v>470</v>
@@ -3135,13 +3497,16 @@
         <v>25</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+      <c r="U96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97">
         <f>A2*'COM-TC'!A32+Samlet!A2*'COM-TC'!A35+Samlet!E2*Dev!A29+Samlet!G2*USB!A21+Samlet!B2*CPU!A13+Samlet!C2*Dash!A26+Samlet!E2*Dev!A30+Samlet!F2*Tele!A13+Samlet!G2*USB!A22</f>
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B97">
         <v>499</v>
@@ -3153,13 +3518,16 @@
         <v>25</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+      <c r="U97">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98">
         <f>A2*'COM-TC'!A37</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B98">
         <v>560</v>
@@ -3171,13 +3539,16 @@
         <v>25</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+      <c r="U98">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99">
         <f>C2*Dash!A29+Samlet!E2*Dev!A31</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B99">
         <v>931</v>
@@ -3189,13 +3560,16 @@
         <v>25</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+      <c r="U99">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100">
         <f>A2*'COM-TC'!A42+Samlet!E2*Dev!A32+Samlet!G2*USB!A23</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B100">
         <v>976</v>
@@ -3207,13 +3581,16 @@
         <v>25</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+      <c r="U100">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101">
         <f>A2*'COM-TC'!A10+Samlet!F2*Tele!A8+Samlet!G2*USB!A16</f>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B101" t="s">
         <v>28</v>
@@ -3225,13 +3602,16 @@
         <v>25</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+      <c r="U101">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102">
         <f>A2*'COM-TC'!A12+Samlet!C2*Dash!A9</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B102" t="s">
         <v>33</v>
@@ -3243,13 +3623,16 @@
         <v>25</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+      <c r="U102">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103">
         <f>G2*USB!A17</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B103" t="s">
         <v>190</v>
@@ -3261,13 +3644,16 @@
         <v>25</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+      <c r="U103">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104">
         <f>A2*'COM-TC'!A16+Samlet!C2*Dash!A13+Samlet!H2*'H-Bridge'!A3</f>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B104" t="s">
         <v>38</v>
@@ -3279,13 +3665,16 @@
         <v>25</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+      <c r="U104">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105">
         <f>G2*USB!A18</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B105" t="s">
         <v>191</v>
@@ -3297,13 +3686,16 @@
         <v>25</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+      <c r="U105">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106">
         <f>A2*'COM-TC'!A18</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B106" t="s">
         <v>40</v>
@@ -3315,13 +3707,16 @@
         <v>25</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+      <c r="U106">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107">
         <f>A2*'COM-TC'!A19</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B107" t="s">
         <v>41</v>
@@ -3333,13 +3728,16 @@
         <v>25</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>344</v>
+      </c>
+      <c r="U107">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108">
         <f>A2*'COM-TC'!A22+Samlet!C2*Dash!A18</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B108" t="s">
         <v>43</v>
@@ -3351,13 +3749,16 @@
         <v>25</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="U108">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109">
         <f>A2*'COM-TC'!A23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B109" t="s">
         <v>44</v>
@@ -3369,13 +3770,16 @@
         <v>25</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+      <c r="U109">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110">
         <f>A2*'COM-TC'!A25+Samlet!C2*Dash!A20</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B110" t="s">
         <v>48</v>
@@ -3387,13 +3791,16 @@
         <v>25</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>323</v>
+      </c>
+      <c r="U110">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111">
         <f>A2*'COM-TC'!A27</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B111" t="s">
         <v>51</v>
@@ -3405,13 +3812,16 @@
         <v>25</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+      <c r="U111">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112">
         <f>C2*Dash!A21</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B112" t="s">
         <v>140</v>
@@ -3425,11 +3835,14 @@
       <c r="E112" s="3" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="U112">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A113">
         <f>A2*'COM-TC'!A34+Samlet!E2*Dev!A33</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B113" t="s">
         <v>58</v>
@@ -3441,13 +3854,16 @@
         <v>25</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+      <c r="U113">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A114">
         <f>A2*'COM-TC'!A36</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B114" t="s">
         <v>59</v>
@@ -3459,13 +3875,16 @@
         <v>25</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+      <c r="U114">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A115">
         <f>A2*'COM-TC'!A40+Samlet!C2*Dash!A28</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B115" t="s">
         <v>61</v>
@@ -3477,13 +3896,16 @@
         <v>25</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+        <v>327</v>
+      </c>
+      <c r="U115">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A116">
         <f>A2*'COM-TC'!A41</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B116" t="s">
         <v>62</v>
@@ -3495,13 +3917,16 @@
         <v>25</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+      <c r="U116">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A117">
         <f>A2*'COM-TC'!A11</f>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B117" t="s">
         <v>30</v>
@@ -3513,13 +3938,16 @@
         <v>32</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+      <c r="U117">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A118">
         <f>C2*Dash!A10</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B118" t="s">
         <v>137</v>
@@ -3531,13 +3959,16 @@
         <v>32</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+      <c r="U118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119">
         <f>A2*'COM-TC'!A26</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B119" t="s">
         <v>49</v>
@@ -3549,13 +3980,16 @@
         <v>1206</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+      <c r="U119">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A120">
         <f>E2*Dev!A34</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C120" t="s">
         <v>174</v>
@@ -3564,13 +3998,16 @@
         <v>175</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+      <c r="U120">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A121">
         <f>C2*Dash!A38</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B121" t="s">
         <v>149</v>
@@ -3582,13 +4019,16 @@
         <v>149</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+      <c r="U121">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A122">
         <f>A2*'COM-TC'!A58+Samlet!C2*Dash!A39+Samlet!E2*Dev!A35</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B122" t="s">
         <v>92</v>
@@ -3600,13 +4040,19 @@
         <v>74</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+        <v>296</v>
+      </c>
+      <c r="U122">
+        <v>10</v>
+      </c>
+      <c r="X122" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A123">
         <f>G2*USB!A24</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B123" t="s">
         <v>200</v>
@@ -3618,13 +4064,16 @@
         <v>201</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+      <c r="U123">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A124">
         <f>A2*'COM-TC'!A59+Samlet!C2*Dash!A40+Samlet!E2*Dev!A36</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B124" t="s">
         <v>93</v>
@@ -3636,13 +4085,19 @@
         <v>94</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+        <v>335</v>
+      </c>
+      <c r="U124">
+        <v>15</v>
+      </c>
+      <c r="X124" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A125">
         <f>B2*CPU!A4</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C125" t="s">
         <v>107</v>
@@ -3651,13 +4106,22 @@
         <v>108</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+      <c r="S125" t="s">
+        <v>336</v>
+      </c>
+      <c r="U125">
+        <v>8</v>
+      </c>
+      <c r="X125" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="126" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A126">
         <f>A2*'COM-TC'!A62</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B126" t="s">
         <v>99</v>
@@ -3668,11 +4132,14 @@
       <c r="D126" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="U126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A127">
         <f>A2*'COM-TC'!A4+Samlet!C2*Dash!A6+Samlet!D2*Debug!A6+Samlet!E2*Dev!A37</f>
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C127" t="s">
         <v>16</v>
@@ -3681,13 +4148,16 @@
         <v>17</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+      <c r="U127">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A128">
         <f>C2*Dash!A42+Samlet!E2*Dev!A38</f>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B128" t="s">
         <v>150</v>
@@ -3699,13 +4169,16 @@
         <v>151</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="U128">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A129">
         <f>B2*CPU!A18+Samlet!G2*USB!A25</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B129" t="s">
         <v>130</v>
@@ -3717,13 +4190,19 @@
         <v>131</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+      <c r="U129">
+        <v>13</v>
+      </c>
+      <c r="X129" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A130">
         <f>A2*'COM-TC'!A64+Samlet!C2*Dash!A43</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B130" t="s">
         <v>102</v>
@@ -3735,13 +4214,19 @@
         <v>74</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+      <c r="U130">
+        <v>7</v>
+      </c>
+      <c r="X130" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="131" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A131">
         <f>A2*'COM-TC'!A5</f>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C131" t="s">
         <v>18</v>
@@ -3750,13 +4235,16 @@
         <v>19</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+      <c r="U131">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="132" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A132">
         <f>G2*USB!A26</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B132" t="s">
         <v>202</v>
@@ -3768,13 +4256,19 @@
         <v>203</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+      <c r="U132">
+        <v>3</v>
+      </c>
+      <c r="X132" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A133">
         <f>E2*Dev!A39</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B133" t="s">
         <v>182</v>
@@ -3786,13 +4280,16 @@
         <v>182</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+      <c r="U133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A134">
         <f>A2*'COM-TC'!A6+Samlet!E2*Dev!A40+Samlet!F2*Tele!A6</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C134" t="s">
         <v>20</v>
@@ -3801,13 +4298,16 @@
         <v>21</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+      <c r="U134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A135">
         <f>C2*Dash!A44</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B135" t="s">
         <v>152</v>
@@ -3819,7 +4319,32 @@
         <v>154</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>354</v>
+        <v>332</v>
+      </c>
+      <c r="U135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>15</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="U136">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>350</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="U138">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -3838,124 +4363,110 @@
     <hyperlink ref="E14" r:id="rId9"/>
     <hyperlink ref="E16" r:id="rId10"/>
     <hyperlink ref="E17" r:id="rId11"/>
-    <hyperlink ref="E18" r:id="rId12"/>
-    <hyperlink ref="E19" r:id="rId13"/>
-    <hyperlink ref="E20" r:id="rId14"/>
-    <hyperlink ref="E21" r:id="rId15"/>
-    <hyperlink ref="E22" r:id="rId16"/>
-    <hyperlink ref="E23" r:id="rId17"/>
-    <hyperlink ref="E24" r:id="rId18"/>
-    <hyperlink ref="E25" r:id="rId19"/>
-    <hyperlink ref="E26" r:id="rId20"/>
-    <hyperlink ref="E27" r:id="rId21"/>
-    <hyperlink ref="E28" r:id="rId22"/>
-    <hyperlink ref="E29" r:id="rId23"/>
-    <hyperlink ref="E30" r:id="rId24"/>
-    <hyperlink ref="E31" r:id="rId25"/>
-    <hyperlink ref="E32" r:id="rId26"/>
-    <hyperlink ref="E33" r:id="rId27"/>
-    <hyperlink ref="E34" r:id="rId28"/>
-    <hyperlink ref="E35" r:id="rId29"/>
-    <hyperlink ref="E36" r:id="rId30"/>
-    <hyperlink ref="E37" r:id="rId31"/>
-    <hyperlink ref="E38" r:id="rId32"/>
-    <hyperlink ref="E39" r:id="rId33"/>
-    <hyperlink ref="E40" r:id="rId34"/>
-    <hyperlink ref="E41" r:id="rId35"/>
-    <hyperlink ref="E42" r:id="rId36"/>
-    <hyperlink ref="E43" r:id="rId37"/>
-    <hyperlink ref="E44" r:id="rId38"/>
-    <hyperlink ref="E45" r:id="rId39"/>
-    <hyperlink ref="E46" r:id="rId40"/>
-    <hyperlink ref="E47" r:id="rId41"/>
-    <hyperlink ref="E48" r:id="rId42"/>
-    <hyperlink ref="E49" r:id="rId43"/>
-    <hyperlink ref="E50" r:id="rId44"/>
-    <hyperlink ref="E51" r:id="rId45"/>
-    <hyperlink ref="E52" r:id="rId46"/>
-    <hyperlink ref="E53" r:id="rId47"/>
-    <hyperlink ref="E54" r:id="rId48"/>
-    <hyperlink ref="E55" r:id="rId49"/>
-    <hyperlink ref="E56" r:id="rId50"/>
-    <hyperlink ref="E57" r:id="rId51"/>
-    <hyperlink ref="E58" r:id="rId52"/>
-    <hyperlink ref="E59" r:id="rId53"/>
-    <hyperlink ref="E60" r:id="rId54"/>
-    <hyperlink ref="E61" r:id="rId55"/>
-    <hyperlink ref="E62" r:id="rId56"/>
-    <hyperlink ref="E63" r:id="rId57"/>
-    <hyperlink ref="E64" r:id="rId58"/>
-    <hyperlink ref="E65" r:id="rId59"/>
-    <hyperlink ref="E66" r:id="rId60"/>
-    <hyperlink ref="E67" r:id="rId61"/>
-    <hyperlink ref="E68" r:id="rId62"/>
-    <hyperlink ref="E69" r:id="rId63"/>
-    <hyperlink ref="E70" r:id="rId64"/>
-    <hyperlink ref="E71" r:id="rId65"/>
-    <hyperlink ref="E72" r:id="rId66"/>
-    <hyperlink ref="E73" r:id="rId67"/>
-    <hyperlink ref="E74" r:id="rId68"/>
-    <hyperlink ref="E75" r:id="rId69"/>
-    <hyperlink ref="E76" r:id="rId70"/>
-    <hyperlink ref="E77" r:id="rId71"/>
-    <hyperlink ref="E78" r:id="rId72"/>
-    <hyperlink ref="E79" r:id="rId73"/>
-    <hyperlink ref="E80" r:id="rId74"/>
-    <hyperlink ref="E81" r:id="rId75"/>
-    <hyperlink ref="E82" r:id="rId76"/>
-    <hyperlink ref="E83" r:id="rId77"/>
-    <hyperlink ref="E84" r:id="rId78"/>
-    <hyperlink ref="E85" r:id="rId79"/>
-    <hyperlink ref="E86" r:id="rId80"/>
-    <hyperlink ref="E87" r:id="rId81"/>
-    <hyperlink ref="E88" r:id="rId82"/>
-    <hyperlink ref="E120" r:id="rId83"/>
-    <hyperlink ref="E121" r:id="rId84"/>
-    <hyperlink ref="E122" r:id="rId85"/>
-    <hyperlink ref="E123" r:id="rId86"/>
-    <hyperlink ref="E125" r:id="rId87"/>
-    <hyperlink ref="E128" r:id="rId88"/>
-    <hyperlink ref="E129" r:id="rId89"/>
-    <hyperlink ref="E130" r:id="rId90"/>
-    <hyperlink ref="E132" r:id="rId91"/>
-    <hyperlink ref="E133" r:id="rId92"/>
-    <hyperlink ref="E89" r:id="rId93"/>
-    <hyperlink ref="E90" r:id="rId94"/>
-    <hyperlink ref="E91" r:id="rId95"/>
-    <hyperlink ref="E92" r:id="rId96"/>
-    <hyperlink ref="E93" r:id="rId97"/>
-    <hyperlink ref="E94" r:id="rId98"/>
-    <hyperlink ref="E95" r:id="rId99"/>
-    <hyperlink ref="E96" r:id="rId100"/>
-    <hyperlink ref="E97" r:id="rId101"/>
-    <hyperlink ref="E98" r:id="rId102"/>
-    <hyperlink ref="E99" r:id="rId103"/>
-    <hyperlink ref="E100" r:id="rId104"/>
-    <hyperlink ref="E101" r:id="rId105"/>
-    <hyperlink ref="E102" r:id="rId106"/>
-    <hyperlink ref="E103" r:id="rId107"/>
-    <hyperlink ref="E104" r:id="rId108"/>
-    <hyperlink ref="E105" r:id="rId109"/>
-    <hyperlink ref="E106" r:id="rId110"/>
-    <hyperlink ref="E107" r:id="rId111"/>
-    <hyperlink ref="E108" r:id="rId112"/>
-    <hyperlink ref="E109" r:id="rId113"/>
-    <hyperlink ref="E110" r:id="rId114"/>
-    <hyperlink ref="E112" r:id="rId115"/>
-    <hyperlink ref="E113" r:id="rId116"/>
-    <hyperlink ref="E114" r:id="rId117"/>
-    <hyperlink ref="E115" r:id="rId118"/>
-    <hyperlink ref="E116" r:id="rId119"/>
-    <hyperlink ref="E117" r:id="rId120"/>
-    <hyperlink ref="E118" r:id="rId121"/>
-    <hyperlink ref="E119" r:id="rId122"/>
-    <hyperlink ref="E127" r:id="rId123"/>
-    <hyperlink ref="E135" r:id="rId124"/>
-    <hyperlink ref="E134" r:id="rId125"/>
-    <hyperlink ref="E131" r:id="rId126"/>
+    <hyperlink ref="E19" r:id="rId12"/>
+    <hyperlink ref="E20" r:id="rId13"/>
+    <hyperlink ref="E23" r:id="rId14"/>
+    <hyperlink ref="E24" r:id="rId15"/>
+    <hyperlink ref="E25" r:id="rId16"/>
+    <hyperlink ref="E26" r:id="rId17"/>
+    <hyperlink ref="E27" r:id="rId18"/>
+    <hyperlink ref="E28" r:id="rId19"/>
+    <hyperlink ref="E29" r:id="rId20"/>
+    <hyperlink ref="E30" r:id="rId21"/>
+    <hyperlink ref="E31" r:id="rId22"/>
+    <hyperlink ref="E32" r:id="rId23"/>
+    <hyperlink ref="E33" r:id="rId24"/>
+    <hyperlink ref="E34" r:id="rId25"/>
+    <hyperlink ref="E35" r:id="rId26"/>
+    <hyperlink ref="E36" r:id="rId27"/>
+    <hyperlink ref="E37" r:id="rId28"/>
+    <hyperlink ref="E38" r:id="rId29"/>
+    <hyperlink ref="E41" r:id="rId30"/>
+    <hyperlink ref="E42" r:id="rId31"/>
+    <hyperlink ref="E43" r:id="rId32"/>
+    <hyperlink ref="E44" r:id="rId33"/>
+    <hyperlink ref="E45" r:id="rId34"/>
+    <hyperlink ref="E47" r:id="rId35"/>
+    <hyperlink ref="E48" r:id="rId36"/>
+    <hyperlink ref="E49" r:id="rId37"/>
+    <hyperlink ref="E55" r:id="rId38"/>
+    <hyperlink ref="E56" r:id="rId39"/>
+    <hyperlink ref="E57" r:id="rId40"/>
+    <hyperlink ref="E58" r:id="rId41"/>
+    <hyperlink ref="E59" r:id="rId42"/>
+    <hyperlink ref="E60" r:id="rId43"/>
+    <hyperlink ref="E61" r:id="rId44"/>
+    <hyperlink ref="E63" r:id="rId45"/>
+    <hyperlink ref="E64" r:id="rId46"/>
+    <hyperlink ref="E65" r:id="rId47"/>
+    <hyperlink ref="E66" r:id="rId48"/>
+    <hyperlink ref="E67" r:id="rId49"/>
+    <hyperlink ref="E68" r:id="rId50"/>
+    <hyperlink ref="E70" r:id="rId51"/>
+    <hyperlink ref="E71" r:id="rId52"/>
+    <hyperlink ref="E72" r:id="rId53"/>
+    <hyperlink ref="E73" r:id="rId54"/>
+    <hyperlink ref="E74" r:id="rId55"/>
+    <hyperlink ref="E75" r:id="rId56"/>
+    <hyperlink ref="E76" r:id="rId57"/>
+    <hyperlink ref="E78" r:id="rId58"/>
+    <hyperlink ref="E79" r:id="rId59"/>
+    <hyperlink ref="E80" r:id="rId60"/>
+    <hyperlink ref="E81" r:id="rId61"/>
+    <hyperlink ref="E82" r:id="rId62"/>
+    <hyperlink ref="E83" r:id="rId63"/>
+    <hyperlink ref="E84" r:id="rId64"/>
+    <hyperlink ref="E88" r:id="rId65"/>
+    <hyperlink ref="E120" r:id="rId66"/>
+    <hyperlink ref="E121" r:id="rId67"/>
+    <hyperlink ref="E122" r:id="rId68"/>
+    <hyperlink ref="E123" r:id="rId69"/>
+    <hyperlink ref="E125" r:id="rId70"/>
+    <hyperlink ref="E128" r:id="rId71"/>
+    <hyperlink ref="E129" r:id="rId72"/>
+    <hyperlink ref="E130" r:id="rId73"/>
+    <hyperlink ref="E132" r:id="rId74"/>
+    <hyperlink ref="E133" r:id="rId75"/>
+    <hyperlink ref="E89" r:id="rId76"/>
+    <hyperlink ref="E90" r:id="rId77"/>
+    <hyperlink ref="E92" r:id="rId78"/>
+    <hyperlink ref="E93" r:id="rId79"/>
+    <hyperlink ref="E94" r:id="rId80"/>
+    <hyperlink ref="E95" r:id="rId81"/>
+    <hyperlink ref="E96" r:id="rId82"/>
+    <hyperlink ref="E97" r:id="rId83"/>
+    <hyperlink ref="E98" r:id="rId84"/>
+    <hyperlink ref="E99" r:id="rId85"/>
+    <hyperlink ref="E100" r:id="rId86"/>
+    <hyperlink ref="E101" r:id="rId87"/>
+    <hyperlink ref="E102" r:id="rId88"/>
+    <hyperlink ref="E103" r:id="rId89"/>
+    <hyperlink ref="E104" r:id="rId90"/>
+    <hyperlink ref="E105" r:id="rId91"/>
+    <hyperlink ref="E108" r:id="rId92"/>
+    <hyperlink ref="E109" r:id="rId93"/>
+    <hyperlink ref="E110" r:id="rId94"/>
+    <hyperlink ref="E113" r:id="rId95"/>
+    <hyperlink ref="E114" r:id="rId96"/>
+    <hyperlink ref="E115" r:id="rId97"/>
+    <hyperlink ref="E116" r:id="rId98"/>
+    <hyperlink ref="E117" r:id="rId99"/>
+    <hyperlink ref="E119" r:id="rId100"/>
+    <hyperlink ref="E127" r:id="rId101"/>
+    <hyperlink ref="E135" r:id="rId102"/>
+    <hyperlink ref="E134" r:id="rId103"/>
+    <hyperlink ref="E131" r:id="rId104"/>
+    <hyperlink ref="E6" r:id="rId105"/>
+    <hyperlink ref="E124" r:id="rId106"/>
+    <hyperlink ref="E39" r:id="rId107"/>
+    <hyperlink ref="E111" r:id="rId108"/>
+    <hyperlink ref="E136" r:id="rId109" display="https://dk.rs-online.com/web/p/printstik-huse/2332753/?searchTerm=233-2753&amp;relevancy-data=636F3D3126696E3D4931384E525353746F636B4E756D6265724D504E266C753D656E266D6D3D6D61746368616C6C26706D3D5E283F69292852537C5253207C52532D293F5C647B337D285C73293F5B5C732D2F255C2E2C5D285C73293F5C647B332C347D2426706F3D313426736E3D592673743D52535F53544F434B5F4E554D4245522677633D4E4F4E45267573743D3233332D32373533267374613D3233333237353326"/>
+    <hyperlink ref="E138" r:id="rId110"/>
+    <hyperlink ref="E21" r:id="rId111"/>
+    <hyperlink ref="E40" r:id="rId112"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId127"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId113"/>
 </worksheet>
 </file>
 
@@ -4118,8 +4629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4651,7 +5162,7 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
         <f>(A2*'COM-TC'!A31)+(Samlet!C2*Dash!A25)</f>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B39">
         <v>60</v>
@@ -5300,8 +5811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6096,8 +6607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6901,8 +7412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>